<commit_message>
Add from_find and to_find keywords
</commit_message>
<xml_diff>
--- a/spec/data/datafile2.xlsx
+++ b/spec/data/datafile2.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="34">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -58,6 +58,9 @@
     <t xml:space="preserve">The Matrix</t>
   </si>
   <si>
+    <t xml:space="preserve">tipo</t>
+  </si>
+  <si>
     <t xml:space="preserve">desde id</t>
   </si>
   <si>
@@ -104,6 +107,24 @@
   </si>
   <si>
     <t xml:space="preserve">restaurant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uuid1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DOES_ONE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uuid2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DOES_TWO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uuid3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DOES_THREE</t>
   </si>
 </sst>
 </file>
@@ -215,7 +236,7 @@
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -272,7 +293,7 @@
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -318,7 +339,7 @@
       <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -358,13 +379,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -380,33 +401,36 @@
         <v>14</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>16</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>17</v>
+      <c r="J1" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="B2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>19</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>20</v>
@@ -414,7 +438,10 @@
       <c r="F2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="1" t="n">
+      <c r="G2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" s="1" t="n">
         <v>1994</v>
       </c>
     </row>
@@ -422,22 +449,25 @@
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>19</v>
+      <c r="B3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H3" s="1" t="n">
+      <c r="H3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" s="1" t="n">
         <v>1993</v>
       </c>
     </row>
@@ -445,20 +475,83 @@
       <c r="A4" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>22</v>
+      <c r="B4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="I4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>26</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I5" s="1" t="n">
+        <v>1983</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I6" s="1" t="n">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B7" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <v>2020</v>
       </c>
     </row>
   </sheetData>

</xml_diff>